<commit_message>
Replaced uploaded category-levelIA xlsx file
</commit_message>
<xml_diff>
--- a/3 mmr land cover transitions/mangroves/intensity analysis/macros/Category_Level_Intensity_Analysis.xlsx
+++ b/3 mmr land cover transitions/mangroves/intensity analysis/macros/Category_Level_Intensity_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dondealban/Dropbox/Research/myanmar/3 mmr land cover transitions/mangroves/intensity analysis/macros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6187D5CC-9E3F-D745-B0FE-B15EAE1F1636}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339B2D7D-CA81-BB41-B3D8-03DA5B7FBFF6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{CA671BDF-03DA-494D-BC2C-3CBDB646B70E}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="28">
   <si>
     <t>BRG</t>
   </si>
@@ -75,54 +75,6 @@
   </si>
   <si>
     <t>2007-2016</t>
-  </si>
-  <si>
-    <t>1996-2008</t>
-  </si>
-  <si>
-    <t>1996-2009</t>
-  </si>
-  <si>
-    <t>1996-2010</t>
-  </si>
-  <si>
-    <t>1996-2011</t>
-  </si>
-  <si>
-    <t>1996-2012</t>
-  </si>
-  <si>
-    <t>1996-2013</t>
-  </si>
-  <si>
-    <t>1996-2014</t>
-  </si>
-  <si>
-    <t>1996-2015</t>
-  </si>
-  <si>
-    <t>2007-2017</t>
-  </si>
-  <si>
-    <t>2007-2018</t>
-  </si>
-  <si>
-    <t>2007-2019</t>
-  </si>
-  <si>
-    <t>2007-2020</t>
-  </si>
-  <si>
-    <t>2007-2021</t>
-  </si>
-  <si>
-    <t>2007-2022</t>
-  </si>
-  <si>
-    <t>2007-2023</t>
-  </si>
-  <si>
-    <t>2007-2024</t>
   </si>
   <si>
     <t>Interval*</t>
@@ -695,37 +647,37 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -765,7 +717,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -800,7 +752,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -835,7 +787,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -870,7 +822,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
@@ -905,7 +857,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>
@@ -940,7 +892,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3">
         <v>7</v>
@@ -975,7 +927,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3">
         <v>8</v>
@@ -1010,7 +962,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3">
         <v>9</v>
@@ -1080,7 +1032,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
@@ -1115,7 +1067,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3">
         <v>3</v>
@@ -1150,7 +1102,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3">
         <v>4</v>
@@ -1185,7 +1137,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3">
         <v>5</v>
@@ -1220,7 +1172,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B16" s="3">
         <v>6</v>
@@ -1255,7 +1207,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B17" s="3">
         <v>7</v>
@@ -1290,7 +1242,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B18" s="3">
         <v>8</v>
@@ -1325,7 +1277,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B19" s="3">
         <v>9</v>
@@ -1391,38 +1343,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>27</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1462,7 +1414,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -1497,7 +1449,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -1532,7 +1484,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -1567,7 +1519,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
@@ -1602,7 +1554,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>
@@ -1637,7 +1589,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3">
         <v>7</v>
@@ -1672,7 +1624,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3">
         <v>8</v>
@@ -1707,7 +1659,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3">
         <v>9</v>
@@ -1777,7 +1729,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
@@ -1812,7 +1764,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3">
         <v>3</v>
@@ -1847,7 +1799,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3">
         <v>4</v>
@@ -1882,7 +1834,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3">
         <v>5</v>
@@ -1917,7 +1869,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B16" s="3">
         <v>6</v>
@@ -1952,7 +1904,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B17" s="3">
         <v>7</v>
@@ -1987,7 +1939,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B18" s="3">
         <v>8</v>
@@ -2022,7 +1974,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B19" s="3">
         <v>9</v>
@@ -2087,37 +2039,37 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -2157,7 +2109,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -2192,7 +2144,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -2227,7 +2179,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -2262,7 +2214,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
@@ -2297,7 +2249,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>
@@ -2332,7 +2284,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3">
         <v>7</v>
@@ -2367,7 +2319,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3">
         <v>8</v>
@@ -2402,7 +2354,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3">
         <v>9</v>
@@ -2472,7 +2424,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
@@ -2507,7 +2459,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3">
         <v>3</v>
@@ -2542,7 +2494,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3">
         <v>4</v>
@@ -2577,7 +2529,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3">
         <v>5</v>
@@ -2612,7 +2564,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B16" s="3">
         <v>6</v>
@@ -2647,7 +2599,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B17" s="3">
         <v>7</v>
@@ -2682,7 +2634,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B18" s="3">
         <v>8</v>
@@ -2717,7 +2669,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B19" s="3">
         <v>9</v>
@@ -2782,38 +2734,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>27</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -2853,7 +2805,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -2888,7 +2840,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -2923,7 +2875,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -2958,7 +2910,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
@@ -2993,7 +2945,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>
@@ -3028,7 +2980,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3">
         <v>7</v>
@@ -3063,7 +3015,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3">
         <v>8</v>
@@ -3098,7 +3050,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3">
         <v>9</v>
@@ -3168,7 +3120,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
@@ -3203,7 +3155,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3">
         <v>3</v>
@@ -3238,7 +3190,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3">
         <v>4</v>
@@ -3273,7 +3225,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3">
         <v>5</v>
@@ -3308,7 +3260,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B16" s="3">
         <v>6</v>
@@ -3343,7 +3295,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B17" s="3">
         <v>7</v>
@@ -3378,7 +3330,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B18" s="3">
         <v>8</v>
@@ -3413,7 +3365,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B19" s="3">
         <v>9</v>
@@ -3477,38 +3429,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>27</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -3548,7 +3500,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -3583,7 +3535,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -3618,7 +3570,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -3653,7 +3605,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
@@ -3688,7 +3640,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>
@@ -3723,7 +3675,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3">
         <v>7</v>
@@ -3758,7 +3710,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3">
         <v>8</v>
@@ -3793,7 +3745,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3">
         <v>9</v>
@@ -3863,7 +3815,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
@@ -3898,7 +3850,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3">
         <v>3</v>
@@ -3933,7 +3885,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3">
         <v>4</v>
@@ -3968,7 +3920,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3">
         <v>5</v>
@@ -4003,7 +3955,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B16" s="3">
         <v>6</v>
@@ -4038,7 +3990,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B17" s="3">
         <v>7</v>
@@ -4073,7 +4025,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B18" s="3">
         <v>8</v>
@@ -4108,7 +4060,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B19" s="3">
         <v>9</v>
@@ -4173,37 +4125,37 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -4243,7 +4195,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -4278,7 +4230,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -4313,7 +4265,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -4348,7 +4300,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
@@ -4383,7 +4335,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>
@@ -4418,7 +4370,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3">
         <v>7</v>
@@ -4453,7 +4405,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3">
         <v>8</v>
@@ -4488,7 +4440,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3">
         <v>9</v>
@@ -4558,7 +4510,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
@@ -4593,7 +4545,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3">
         <v>3</v>
@@ -4628,7 +4580,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3">
         <v>4</v>
@@ -4663,7 +4615,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3">
         <v>5</v>
@@ -4698,7 +4650,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B16" s="3">
         <v>6</v>
@@ -4733,7 +4685,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B17" s="3">
         <v>7</v>
@@ -4768,7 +4720,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B18" s="3">
         <v>8</v>
@@ -4803,7 +4755,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B19" s="3">
         <v>9</v>
@@ -4868,38 +4820,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>27</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -4939,7 +4891,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -4974,7 +4926,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -5009,7 +4961,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -5044,7 +4996,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
@@ -5079,7 +5031,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>
@@ -5114,7 +5066,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3">
         <v>7</v>
@@ -5149,7 +5101,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3">
         <v>8</v>
@@ -5184,7 +5136,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3">
         <v>9</v>
@@ -5254,7 +5206,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
@@ -5289,7 +5241,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3">
         <v>3</v>
@@ -5324,7 +5276,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3">
         <v>4</v>
@@ -5359,7 +5311,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3">
         <v>5</v>
@@ -5394,7 +5346,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B16" s="3">
         <v>6</v>
@@ -5429,7 +5381,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B17" s="3">
         <v>7</v>
@@ -5464,7 +5416,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B18" s="3">
         <v>8</v>
@@ -5499,7 +5451,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B19" s="3">
         <v>9</v>
@@ -5564,37 +5516,37 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -5634,7 +5586,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -5669,7 +5621,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -5704,7 +5656,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -5739,7 +5691,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
@@ -5774,7 +5726,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>
@@ -5809,7 +5761,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3">
         <v>7</v>
@@ -5844,7 +5796,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3">
         <v>8</v>
@@ -5879,7 +5831,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3">
         <v>9</v>
@@ -5949,7 +5901,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
@@ -5984,7 +5936,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3">
         <v>3</v>
@@ -6019,7 +5971,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3">
         <v>4</v>
@@ -6054,7 +6006,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3">
         <v>5</v>
@@ -6089,7 +6041,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B16" s="3">
         <v>6</v>
@@ -6124,7 +6076,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B17" s="3">
         <v>7</v>
@@ -6159,7 +6111,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B18" s="3">
         <v>8</v>
@@ -6194,7 +6146,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B19" s="3">
         <v>9</v>
@@ -6259,38 +6211,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>27</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -6330,7 +6282,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -6365,7 +6317,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -6400,7 +6352,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -6435,7 +6387,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
@@ -6470,7 +6422,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>
@@ -6505,7 +6457,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3">
         <v>7</v>
@@ -6540,7 +6492,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3">
         <v>8</v>
@@ -6575,7 +6527,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3">
         <v>9</v>
@@ -6645,7 +6597,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
@@ -6680,7 +6632,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3">
         <v>3</v>
@@ -6715,7 +6667,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3">
         <v>4</v>
@@ -6750,7 +6702,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3">
         <v>5</v>
@@ -6785,7 +6737,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B16" s="3">
         <v>6</v>
@@ -6820,7 +6772,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B17" s="3">
         <v>7</v>
@@ -6855,7 +6807,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B18" s="3">
         <v>8</v>
@@ -6890,7 +6842,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B19" s="3">
         <v>9</v>
@@ -6955,37 +6907,37 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -7025,7 +6977,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -7060,7 +7012,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -7095,7 +7047,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -7130,7 +7082,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
@@ -7165,7 +7117,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>
@@ -7200,7 +7152,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3">
         <v>7</v>
@@ -7235,7 +7187,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3">
         <v>8</v>
@@ -7270,7 +7222,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3">
         <v>9</v>
@@ -7340,7 +7292,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
@@ -7375,7 +7327,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3">
         <v>3</v>
@@ -7410,7 +7362,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3">
         <v>4</v>
@@ -7445,7 +7397,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3">
         <v>5</v>
@@ -7480,7 +7432,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B16" s="3">
         <v>6</v>
@@ -7515,7 +7467,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B17" s="3">
         <v>7</v>
@@ -7550,7 +7502,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B18" s="3">
         <v>8</v>
@@ -7585,7 +7537,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B19" s="3">
         <v>9</v>
@@ -7650,38 +7602,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>27</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -7721,7 +7673,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -7756,7 +7708,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -7791,7 +7743,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -7826,7 +7778,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
@@ -7861,7 +7813,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>
@@ -7896,7 +7848,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3">
         <v>7</v>
@@ -7931,7 +7883,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3">
         <v>8</v>
@@ -7966,7 +7918,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3">
         <v>9</v>
@@ -8036,7 +7988,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
@@ -8071,7 +8023,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3">
         <v>3</v>
@@ -8106,7 +8058,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3">
         <v>4</v>
@@ -8141,7 +8093,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3">
         <v>5</v>
@@ -8176,7 +8128,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B16" s="3">
         <v>6</v>
@@ -8211,7 +8163,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B17" s="3">
         <v>7</v>
@@ -8246,7 +8198,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B18" s="3">
         <v>8</v>
@@ -8281,7 +8233,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B19" s="3">
         <v>9</v>
@@ -8346,37 +8298,37 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -8416,7 +8368,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -8451,7 +8403,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -8486,7 +8438,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -8521,7 +8473,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
@@ -8556,7 +8508,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>
@@ -8591,7 +8543,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3">
         <v>7</v>
@@ -8626,7 +8578,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3">
         <v>8</v>
@@ -8661,7 +8613,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3">
         <v>9</v>
@@ -8731,7 +8683,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
@@ -8766,7 +8718,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B13" s="3">
         <v>3</v>
@@ -8801,7 +8753,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3">
         <v>4</v>
@@ -8836,7 +8788,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3">
         <v>5</v>
@@ -8871,7 +8823,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B16" s="3">
         <v>6</v>
@@ -8906,7 +8858,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B17" s="3">
         <v>7</v>
@@ -8941,7 +8893,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B18" s="3">
         <v>8</v>
@@ -8976,7 +8928,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B19" s="3">
         <v>9</v>

</xml_diff>